<commit_message>
Update some erroe and Readme
</commit_message>
<xml_diff>
--- a/config/Holdings.xlsx
+++ b/config/Holdings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LabourerLucas\Desktop\Daliy-Stock-Email-Report\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LabourerLucas\Desktop\Daliy-Stock-Email-with-quant\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D668A3-8D5F-4D35-8765-5459B3D37B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7419279A-37CD-4771-829C-716B8EC7FE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Ticker</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,14 +48,6 @@
   </si>
   <si>
     <t>QCOM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PYPL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NVDA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -385,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -445,31 +437,9 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>79.45</v>
+        <v>416.61</v>
       </c>
       <c r="C5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>135</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>416.61</v>
-      </c>
-      <c r="C7">
         <v>3</v>
       </c>
     </row>

</xml_diff>